<commit_message>
excel sheet expanded for tidy data
</commit_message>
<xml_diff>
--- a/Prototypes/PN_1/Lit Review Matrix - Upstream Policies and Health Outcomes 6-28-21.xlsx
+++ b/Prototypes/PN_1/Lit Review Matrix - Upstream Policies and Health Outcomes 6-28-21.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamila Porter\Documents\Urban Health Agenda\Lit Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranli\Desktop\Git local\BCHC Policy Review\Prototypes\PN_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4875F1-09AB-4B25-ADDC-584F684B3C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E597D8-CC92-4491-BA60-EB1DB3AD060E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{91655CBE-7744-41B9-AECB-CA897763B8F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{91655CBE-7744-41B9-AECB-CA897763B8F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="policy group" sheetId="3" r:id="rId3"/>
+    <sheet name="outcome groups" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Chronic diseases</t>
   </si>
@@ -124,13 +127,37 @@
   </si>
   <si>
     <t>Policies related to childcare (e.g., access, affordability, etc.)</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>Policy Group</t>
+  </si>
+  <si>
+    <t>Outcome Group</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Jim Crow birthplace was associated with increased odds of ER− breast cancer only among the black, not white women, with the effect strongest for women born before 1965. Among black women, the odds ratio (OR) for an ER− tumor, comparing women born in a Jim Crow versus not Jim Crow state, equaled 1.09 (95% confidence interval [CI] 1.06, 1.13), on par with the OR comparing women in the worst versus best census tract socioeconomic quintiles (1.15; 95% CI 1.07, 1.23). The black versus white OR for ER− was higher among women born in Jim Crow versus non-Jim Crow states (1.41 [95% CI 1.13, 1.46] vs. 1.27 [95% CI 1.24, 1.31]).</t>
+  </si>
+  <si>
+    <t>Summary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +186,33 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -222,6 +276,49 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,36 +636,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611E71C5-D3CE-45F1-93F6-C02EF4998E77}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="3" customWidth="1"/>
-    <col min="3" max="5" width="14.54296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="4" customWidth="1"/>
-    <col min="7" max="11" width="14.54296875" style="4" customWidth="1"/>
-    <col min="12" max="15" width="11.1796875" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="34.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
+    <col min="3" max="5" width="14.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="4" customWidth="1"/>
+    <col min="7" max="11" width="14.5703125" style="4" customWidth="1"/>
+    <col min="12" max="15" width="11.140625" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -587,7 +684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="27.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
@@ -602,7 +699,7 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -617,7 +714,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -632,7 +729,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -647,7 +744,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -662,7 +759,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
@@ -677,7 +774,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -692,7 +789,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -707,19 +804,19 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="19" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="6"/>
@@ -728,7 +825,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
@@ -743,7 +840,7 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -760,7 +857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -777,7 +874,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
@@ -792,7 +889,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" ht="36.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
@@ -807,7 +904,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -820,26 +917,26 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="27.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="27.6" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C1:L37">
     <sortCondition descending="1" ref="C1:C37"/>
@@ -849,10 +946,306 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76B3283-73AF-4BC5-8FB9-52DC3BCE3176}">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="82" customWidth="1"/>
+    <col min="6" max="7" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="26"/>
+    </row>
+    <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="26"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FF43D0-345F-4973-BAC3-C250ABD5562A}">
+  <dimension ref="B2:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B5:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="44" style="10" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="2:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="2:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="2:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="2:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD2B709-1C92-4CBB-8594-68AFEB29BDA0}">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="18"/>
+    </row>
+    <row r="8" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1079,19 +1472,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354C80EB-C06E-464C-AD3C-7B13542B0A24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB8F18E-5FC7-49C0-8742-4EBD888DA06A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1116,9 +1505,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB8F18E-5FC7-49C0-8742-4EBD888DA06A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354C80EB-C06E-464C-AD3C-7B13542B0A24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tidy data in csv
</commit_message>
<xml_diff>
--- a/Prototypes/PN_1/Lit Review Matrix - Upstream Policies and Health Outcomes 6-28-21.xlsx
+++ b/Prototypes/PN_1/Lit Review Matrix - Upstream Policies and Health Outcomes 6-28-21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranli\Desktop\Git local\BCHC Policy Review\Prototypes\PN_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E597D8-CC92-4491-BA60-EB1DB3AD060E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0260458D-4086-4900-979C-69C8309EF30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{91655CBE-7744-41B9-AECB-CA897763B8F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91655CBE-7744-41B9-AECB-CA897763B8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Chronic diseases</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect Size </t>
+  </si>
+  <si>
+    <t>P-value</t>
   </si>
 </sst>
 </file>
@@ -948,10 +954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76B3283-73AF-4BC5-8FB9-52DC3BCE3176}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +969,7 @@
     <col min="6" max="7" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>30</v>
       </c>
@@ -979,8 +985,14 @@
       <c r="F2" s="25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="G2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
@@ -994,8 +1006,10 @@
         <v>36</v>
       </c>
       <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
         <v>19</v>
       </c>
@@ -1007,8 +1021,10 @@
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="26"/>
-    </row>
-    <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>20</v>
       </c>
@@ -1020,16 +1036,21 @@
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="26"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1157,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD2B709-1C92-4CBB-8594-68AFEB29BDA0}">
   <dimension ref="B2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1249,6 +1270,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B33ACE731AB07341AE5126C3DA9F4C14" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e6ff49344acef95e2064f655fa0c8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="add7b089-4dde-484e-a58b-af385cd258ee" xmlns:ns3="2668201c-984e-41c3-be1f-d1fe4f7774bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="131adc71cac139061e16379c73acc269" ns2:_="" ns3:_="">
     <xsd:import namespace="add7b089-4dde-484e-a58b-af385cd258ee"/>
@@ -1471,12 +1498,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FB8F18E-5FC7-49C0-8742-4EBD888DA06A}">
   <ds:schemaRefs>
@@ -1486,6 +1507,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354C80EB-C06E-464C-AD3C-7B13542B0A24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D69B468-98E1-4AD8-B5C6-1FF56939E88B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1502,13 +1532,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354C80EB-C06E-464C-AD3C-7B13542B0A24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>